<commit_message>
some ex from 4.9 solved
</commit_message>
<xml_diff>
--- a/navidi/Exercises.xlsx
+++ b/navidi/Exercises.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\_Work\Statistics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Others\Statistics\navidi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0529ABD5-5081-47A6-BADF-C075383A1714}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A74397B4-1334-4235-95F3-554A071B448C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4680" yWindow="1460" windowWidth="38400" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="51420" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Exercises" sheetId="1" r:id="rId1"/>
     <sheet name="Normal" sheetId="5" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" calcOnSave="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1224,7 +1224,7 @@
   <dimension ref="A1:AO83"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="O69" sqref="O69"/>
+      <selection activeCell="K72" sqref="K72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3545,13 +3545,13 @@
       <c r="D72" s="1">
         <v>2</v>
       </c>
-      <c r="E72" s="1">
+      <c r="E72" s="4">
         <v>3</v>
       </c>
       <c r="F72" s="1">
         <v>4</v>
       </c>
-      <c r="G72" s="1">
+      <c r="G72" s="4">
         <v>5</v>
       </c>
       <c r="H72" s="1">

</xml_diff>

<commit_message>
5.2 Confidence Intervals for a Population Mean, Variance Unknown
</commit_message>
<xml_diff>
--- a/navidi/Exercises.xlsx
+++ b/navidi/Exercises.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\_Work\Statistics\navidi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6F36092-B154-4E4D-803B-50E61E84A15D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D621A87-99CB-422A-9FF9-E72A266CA867}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2660" yWindow="2660" windowWidth="38400" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5150" yWindow="2650" windowWidth="38400" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Exercises" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="298">
   <si>
     <t>2.2 Counting Methods</t>
   </si>
@@ -908,6 +908,54 @@
   </si>
   <si>
     <t>5.2 Confidence Intervals for a Population Mean, Variance Unknown</t>
+  </si>
+  <si>
+    <t>5.11</t>
+  </si>
+  <si>
+    <t>5.12</t>
+  </si>
+  <si>
+    <t>5.13</t>
+  </si>
+  <si>
+    <t>5.14</t>
+  </si>
+  <si>
+    <t>5.15</t>
+  </si>
+  <si>
+    <t>5.16</t>
+  </si>
+  <si>
+    <t>5.17</t>
+  </si>
+  <si>
+    <t>5.18</t>
+  </si>
+  <si>
+    <t>5.19</t>
+  </si>
+  <si>
+    <t>5.20</t>
+  </si>
+  <si>
+    <t>5.21</t>
+  </si>
+  <si>
+    <t>5.3 Confidence Intervals for Proportions</t>
+  </si>
+  <si>
+    <t>5.22</t>
+  </si>
+  <si>
+    <t>5.23</t>
+  </si>
+  <si>
+    <t>5.24</t>
+  </si>
+  <si>
+    <t>5.4 Confidence Intervals for the Difference Between Two Means</t>
   </si>
 </sst>
 </file>
@@ -2184,10 +2232,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AO88"/>
+  <dimension ref="A1:AO94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="N89" sqref="N89"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="AB75" sqref="AB75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3245,7 +3293,7 @@
       <c r="E30" s="1">
         <v>3</v>
       </c>
-      <c r="F30" s="1">
+      <c r="F30" s="4">
         <v>4</v>
       </c>
       <c r="G30" s="1">
@@ -4699,7 +4747,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="81" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:38" x14ac:dyDescent="0.35">
       <c r="C81" s="1">
         <v>1</v>
       </c>
@@ -4743,12 +4791,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="82" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:38" x14ac:dyDescent="0.35">
       <c r="B82" s="3" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="83" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:38" x14ac:dyDescent="0.35">
       <c r="C83" s="1">
         <v>1</v>
       </c>
@@ -4840,17 +4888,17 @@
         <v>30</v>
       </c>
     </row>
-    <row r="84" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A84" s="3" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="85" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:38" x14ac:dyDescent="0.35">
       <c r="B85" s="3" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="86" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:38" x14ac:dyDescent="0.35">
       <c r="C86" s="1" t="s">
         <v>271</v>
       </c>
@@ -4882,20 +4930,20 @@
         <v>280</v>
       </c>
     </row>
-    <row r="87" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:38" x14ac:dyDescent="0.35">
       <c r="C87" s="1">
         <v>1</v>
       </c>
       <c r="D87" s="1">
         <v>2</v>
       </c>
-      <c r="E87" s="1">
+      <c r="E87" s="4">
         <v>3</v>
       </c>
       <c r="F87" s="1">
         <v>4</v>
       </c>
-      <c r="G87" s="1">
+      <c r="G87" s="4">
         <v>5</v>
       </c>
       <c r="H87" s="1">
@@ -4938,9 +4986,234 @@
         <v>18</v>
       </c>
     </row>
-    <row r="88" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:38" x14ac:dyDescent="0.35">
       <c r="B88" s="3" t="s">
         <v>281</v>
+      </c>
+    </row>
+    <row r="89" spans="1:38" x14ac:dyDescent="0.35">
+      <c r="C89" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="E89" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="F89" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="G89" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="H89" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="I89" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="J89" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="K89" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="L89" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="M89" s="1" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="90" spans="1:38" x14ac:dyDescent="0.35">
+      <c r="C90" s="1">
+        <v>1</v>
+      </c>
+      <c r="D90" s="1">
+        <v>2</v>
+      </c>
+      <c r="E90" s="4">
+        <v>3</v>
+      </c>
+      <c r="F90" s="1">
+        <v>4</v>
+      </c>
+      <c r="G90" s="1">
+        <v>5</v>
+      </c>
+      <c r="H90" s="1">
+        <v>6</v>
+      </c>
+      <c r="I90" s="1">
+        <v>7</v>
+      </c>
+      <c r="J90" s="1">
+        <v>8</v>
+      </c>
+      <c r="K90" s="1">
+        <v>9</v>
+      </c>
+      <c r="L90" s="1">
+        <v>10</v>
+      </c>
+      <c r="M90" s="1">
+        <v>11</v>
+      </c>
+      <c r="N90" s="1">
+        <v>12</v>
+      </c>
+      <c r="O90" s="1">
+        <v>13</v>
+      </c>
+      <c r="P90" s="1">
+        <v>14</v>
+      </c>
+      <c r="Q90" s="1">
+        <v>15</v>
+      </c>
+      <c r="R90" s="1">
+        <v>16</v>
+      </c>
+      <c r="S90" s="1">
+        <v>17</v>
+      </c>
+      <c r="T90" s="1">
+        <v>18</v>
+      </c>
+      <c r="U90" s="1">
+        <v>19</v>
+      </c>
+      <c r="V90" s="1">
+        <v>20</v>
+      </c>
+      <c r="W90" s="1">
+        <v>21</v>
+      </c>
+      <c r="X90" s="1">
+        <v>22</v>
+      </c>
+      <c r="Y90" s="1">
+        <v>23</v>
+      </c>
+      <c r="Z90" s="1">
+        <v>24</v>
+      </c>
+      <c r="AA90" s="1">
+        <v>25</v>
+      </c>
+      <c r="AB90" s="1">
+        <v>26</v>
+      </c>
+      <c r="AC90" s="1">
+        <v>27</v>
+      </c>
+      <c r="AD90" s="1">
+        <v>28</v>
+      </c>
+      <c r="AE90" s="1">
+        <v>29</v>
+      </c>
+      <c r="AF90" s="1">
+        <v>30</v>
+      </c>
+      <c r="AG90" s="1">
+        <v>31</v>
+      </c>
+      <c r="AH90" s="1">
+        <v>32</v>
+      </c>
+      <c r="AI90" s="1">
+        <v>33</v>
+      </c>
+      <c r="AJ90" s="1">
+        <v>34</v>
+      </c>
+      <c r="AK90" s="1">
+        <v>35</v>
+      </c>
+      <c r="AL90" s="1">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="91" spans="1:38" x14ac:dyDescent="0.35">
+      <c r="B91" s="3" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="92" spans="1:38" x14ac:dyDescent="0.35">
+      <c r="C92" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="E92" s="1" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="93" spans="1:38" x14ac:dyDescent="0.35">
+      <c r="C93" s="1">
+        <v>1</v>
+      </c>
+      <c r="D93" s="1">
+        <v>2</v>
+      </c>
+      <c r="E93" s="1">
+        <v>3</v>
+      </c>
+      <c r="F93" s="1">
+        <v>4</v>
+      </c>
+      <c r="G93" s="1">
+        <v>5</v>
+      </c>
+      <c r="H93" s="1">
+        <v>6</v>
+      </c>
+      <c r="I93" s="1">
+        <v>7</v>
+      </c>
+      <c r="J93" s="1">
+        <v>8</v>
+      </c>
+      <c r="K93" s="1">
+        <v>9</v>
+      </c>
+      <c r="L93" s="1">
+        <v>10</v>
+      </c>
+      <c r="M93" s="1">
+        <v>11</v>
+      </c>
+      <c r="N93" s="1">
+        <v>12</v>
+      </c>
+      <c r="O93" s="1">
+        <v>13</v>
+      </c>
+      <c r="P93" s="1">
+        <v>14</v>
+      </c>
+      <c r="Q93" s="1">
+        <v>15</v>
+      </c>
+      <c r="R93" s="1">
+        <v>16</v>
+      </c>
+      <c r="S93" s="1">
+        <v>17</v>
+      </c>
+      <c r="T93" s="1">
+        <v>18</v>
+      </c>
+      <c r="U93" s="1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="94" spans="1:38" x14ac:dyDescent="0.35">
+      <c r="B94" s="3" t="s">
+        <v>297</v>
       </c>
     </row>
   </sheetData>
@@ -4948,7 +5221,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="G6:H6 I6:J6 C9:D9 D20:S22 D15:I17 D26:G26 C25:F25 C28:Y28 C39:F39 L36 C42:J42 K50:L50 C53:O53 C56:L56 C59:I59 J59:P59 C62:F62 C65:I65 C71:E71 C77:I77 C80:K80 C68:F68" twoDigitTextYear="1"/>
+    <ignoredError sqref="G6:H6 I6:J6 C9:D9 D20:S22 D15:I17 D26:G26 C25:F25 C28:Y28 C39:F39 L36 C42:J42 K50:L50 C53:O53 C56:L56 C59:I59 J59:P59 C62:F62 C65:I65 C71:E71 C77:I77 C80:K80 C68:F68 E89:M89 C92:E92" twoDigitTextYear="1"/>
     <ignoredError sqref="C26 C15:C17 C20:C22" twoDigitTextYear="1" numberStoredAsText="1"/>
     <ignoredError sqref="C18:C19 C23:C24 AL21 C34:K34 C72 C75:L75" numberStoredAsText="1"/>
   </ignoredErrors>
@@ -4961,7 +5234,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G56" sqref="G56"/>
+      <selection pane="bottomLeft" activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8377,10 +8650,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B642E4E-4CEB-4761-98FC-68FA36484AD6}">
-  <dimension ref="B3:Y125"/>
+  <dimension ref="B3:X125"/>
   <sheetViews>
     <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q47" sqref="Q47"/>
+      <selection activeCell="R44" sqref="R44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8503,7 +8776,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="17" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:24" x14ac:dyDescent="0.35">
       <c r="D17" s="6" t="s">
         <v>258</v>
       </c>
@@ -8511,7 +8784,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:24" x14ac:dyDescent="0.35">
       <c r="D18" s="6" t="s">
         <v>255</v>
       </c>
@@ -8519,7 +8792,7 @@
         <v>12.05</v>
       </c>
     </row>
-    <row r="19" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:24" x14ac:dyDescent="0.35">
       <c r="D19" s="6" t="s">
         <v>256</v>
       </c>
@@ -8545,7 +8818,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="20" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:24" x14ac:dyDescent="0.35">
       <c r="D20" s="6" t="s">
         <v>257</v>
       </c>
@@ -8583,7 +8856,7 @@
         <v>9.28818501377352E-2</v>
       </c>
     </row>
-    <row r="21" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:24" x14ac:dyDescent="0.35">
       <c r="I21" s="6">
         <v>0.02</v>
       </c>
@@ -8614,7 +8887,7 @@
         <v>0.20850836168401488</v>
       </c>
     </row>
-    <row r="22" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:24" x14ac:dyDescent="0.35">
       <c r="D22" s="6" t="s">
         <v>259</v>
       </c>
@@ -8623,7 +8896,13 @@
         <v>4.7790352272812336E-2</v>
       </c>
     </row>
-    <row r="27" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="X25" s="6">
+        <f>1/(1+0.5*0.97/0.99)</f>
+        <v>0.67118644067796618</v>
+      </c>
+    </row>
+    <row r="27" spans="2:24" x14ac:dyDescent="0.35">
       <c r="B27" s="6">
         <v>0.1</v>
       </c>
@@ -8637,7 +8916,7 @@
         <v>1.18</v>
       </c>
     </row>
-    <row r="28" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:24" x14ac:dyDescent="0.35">
       <c r="B28" s="6">
         <v>0.5</v>
       </c>
@@ -8655,7 +8934,7 @@
         <v>1048576</v>
       </c>
     </row>
-    <row r="29" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:24" x14ac:dyDescent="0.35">
       <c r="B29" s="6">
         <v>0.4</v>
       </c>
@@ -8663,7 +8942,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="30" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:24" x14ac:dyDescent="0.35">
       <c r="H30" s="6">
         <f>H28-H27</f>
         <v>4.7199999999999989</v>
@@ -8673,12 +8952,12 @@
         <v>2.118962010041709</v>
       </c>
     </row>
-    <row r="31" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:24" x14ac:dyDescent="0.35">
       <c r="B31" s="6" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="32" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:24" x14ac:dyDescent="0.35">
       <c r="B32" s="6" t="s">
         <v>267</v>
       </c>
@@ -8686,12 +8965,12 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="33" spans="2:25" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B33" s="6" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="34" spans="2:25" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:18" x14ac:dyDescent="0.35">
       <c r="K34" s="6" t="s">
         <v>258</v>
       </c>
@@ -8706,7 +8985,7 @@
         <v>4.0000000000000008E-2</v>
       </c>
     </row>
-    <row r="35" spans="2:25" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:18" x14ac:dyDescent="0.35">
       <c r="H35" s="6">
         <v>0.1</v>
       </c>
@@ -8724,17 +9003,17 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="36" spans="2:25" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:18" x14ac:dyDescent="0.35">
       <c r="H36" s="6">
         <v>0.25</v>
       </c>
     </row>
-    <row r="37" spans="2:25" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:18" x14ac:dyDescent="0.35">
       <c r="H37" s="6">
         <v>0.45</v>
       </c>
     </row>
-    <row r="38" spans="2:25" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:18" x14ac:dyDescent="0.35">
       <c r="L38" s="6">
         <f>SQRT(L35*N34+((1/4)*L34^2/L35)*N35)</f>
         <v>0.74582169450881497</v>
@@ -8747,32 +9026,20 @@
         <f>L38/N38</f>
         <v>4.7169905660283021E-2</v>
       </c>
-      <c r="T38" s="6">
-        <v>25</v>
-      </c>
-      <c r="U38" s="6">
-        <f>0.2*SQRT(5)</f>
-        <v>0.44721359549995798</v>
-      </c>
-      <c r="W38" s="6">
-        <v>24</v>
-      </c>
-      <c r="X38" s="6">
-        <f>(W38-T38)/U38</f>
-        <v>-2.2360679774997894</v>
-      </c>
-      <c r="Y38" s="6">
-        <f>_xlfn.NORM.S.DIST(X38,TRUE)</f>
-        <v>1.2673659338734137E-2</v>
-      </c>
-    </row>
-    <row r="39" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="R38" s="6">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="39" spans="2:18" x14ac:dyDescent="0.35">
       <c r="H39" s="6">
         <f>SUM(H35:H38)</f>
         <v>0.8</v>
       </c>
-    </row>
-    <row r="40" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="R39" s="6">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="40" spans="2:18" x14ac:dyDescent="0.35">
       <c r="L40" s="6">
         <f>SQRT(L35^2/L34^3*N34+4/L34*N35)</f>
         <v>0.48166378315169184</v>
@@ -8785,8 +9052,18 @@
         <f>L40/N40</f>
         <v>5.3851648071345043E-2</v>
       </c>
-    </row>
-    <row r="42" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="R40" s="6">
+        <f>R38+R39</f>
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="41" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="R41" s="6">
+        <f>R40/2</f>
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="42" spans="2:18" x14ac:dyDescent="0.35">
       <c r="L42" s="6">
         <f>2*SQRT(L34^2*N34+L35^2*N35)</f>
         <v>10.198039027185569</v>
@@ -8799,14 +9076,29 @@
         <f>L42/N42</f>
         <v>8.158431221748455E-2</v>
       </c>
-    </row>
-    <row r="46" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="R42" s="6">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="43" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="R43" s="6">
+        <f>R42-R41</f>
+        <v>7.0000000000000062E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="R44" s="6">
+        <f>R43*SQRT(114)/1.96</f>
+        <v>0.38132422328683291</v>
+      </c>
+    </row>
+    <row r="46" spans="2:18" x14ac:dyDescent="0.35">
       <c r="K46" s="6">
         <f>0.2*SQRT(5)</f>
         <v>0.44721359549995798</v>
       </c>
     </row>
-    <row r="47" spans="2:25" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:18" x14ac:dyDescent="0.35">
       <c r="Q47" s="6">
         <f>(5.06-5)/0.08</f>
         <v>0.74999999999999512</v>

</xml_diff>

<commit_message>
5.4 Confidence Intervals for the Difference Between Two Means
</commit_message>
<xml_diff>
--- a/navidi/Exercises.xlsx
+++ b/navidi/Exercises.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\_Work\Statistics\navidi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D621A87-99CB-422A-9FF9-E72A266CA867}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A69056B2-F53F-492D-8D6D-804AF95415A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5150" yWindow="2650" windowWidth="38400" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18680" yWindow="2510" windowWidth="38400" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Exercises" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="304">
   <si>
     <t>2.2 Counting Methods</t>
   </si>
@@ -956,6 +956,24 @@
   </si>
   <si>
     <t>5.4 Confidence Intervals for the Difference Between Two Means</t>
+  </si>
+  <si>
+    <t>5.25</t>
+  </si>
+  <si>
+    <t>5.26</t>
+  </si>
+  <si>
+    <t>5.27</t>
+  </si>
+  <si>
+    <t>5.28</t>
+  </si>
+  <si>
+    <t>5.29</t>
+  </si>
+  <si>
+    <t>5.5 Confidence Intervals for the Difference Between Two Proportions</t>
   </si>
 </sst>
 </file>
@@ -2232,10 +2250,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AO94"/>
+  <dimension ref="A1:AO97"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="AB75" sqref="AB75"/>
+      <selection activeCell="J108" sqref="J108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4747,7 +4765,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="81" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:41" x14ac:dyDescent="0.35">
       <c r="C81" s="1">
         <v>1</v>
       </c>
@@ -4791,12 +4809,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="82" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:41" x14ac:dyDescent="0.35">
       <c r="B82" s="3" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="83" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:41" x14ac:dyDescent="0.35">
       <c r="C83" s="1">
         <v>1</v>
       </c>
@@ -4888,17 +4906,17 @@
         <v>30</v>
       </c>
     </row>
-    <row r="84" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A84" s="3" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="85" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:41" x14ac:dyDescent="0.35">
       <c r="B85" s="3" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="86" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:41" x14ac:dyDescent="0.35">
       <c r="C86" s="1" t="s">
         <v>271</v>
       </c>
@@ -4930,7 +4948,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="87" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:41" x14ac:dyDescent="0.35">
       <c r="C87" s="1">
         <v>1</v>
       </c>
@@ -4986,12 +5004,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="88" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:41" x14ac:dyDescent="0.35">
       <c r="B88" s="3" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="89" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:41" x14ac:dyDescent="0.35">
       <c r="C89" s="1" t="s">
         <v>282</v>
       </c>
@@ -5026,7 +5044,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="90" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:41" x14ac:dyDescent="0.35">
       <c r="C90" s="1">
         <v>1</v>
       </c>
@@ -5136,12 +5154,12 @@
         <v>36</v>
       </c>
     </row>
-    <row r="91" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:41" x14ac:dyDescent="0.35">
       <c r="B91" s="3" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="92" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:41" x14ac:dyDescent="0.35">
       <c r="C92" s="1" t="s">
         <v>294</v>
       </c>
@@ -5152,7 +5170,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="93" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:41" x14ac:dyDescent="0.35">
       <c r="C93" s="1">
         <v>1</v>
       </c>
@@ -5211,9 +5229,150 @@
         <v>19</v>
       </c>
     </row>
-    <row r="94" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:41" x14ac:dyDescent="0.35">
       <c r="B94" s="3" t="s">
         <v>297</v>
+      </c>
+    </row>
+    <row r="95" spans="1:41" x14ac:dyDescent="0.35">
+      <c r="C95" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="E95" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="F95" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="G95" s="1" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="96" spans="1:41" x14ac:dyDescent="0.35">
+      <c r="C96" s="1">
+        <v>1</v>
+      </c>
+      <c r="D96" s="1">
+        <v>2</v>
+      </c>
+      <c r="E96" s="1">
+        <v>3</v>
+      </c>
+      <c r="F96" s="1">
+        <v>4</v>
+      </c>
+      <c r="G96" s="1">
+        <v>5</v>
+      </c>
+      <c r="H96" s="1">
+        <v>6</v>
+      </c>
+      <c r="I96" s="1">
+        <v>7</v>
+      </c>
+      <c r="J96" s="1">
+        <v>8</v>
+      </c>
+      <c r="K96" s="1">
+        <v>9</v>
+      </c>
+      <c r="L96" s="1">
+        <v>10</v>
+      </c>
+      <c r="M96" s="1">
+        <v>11</v>
+      </c>
+      <c r="N96" s="1">
+        <v>12</v>
+      </c>
+      <c r="O96" s="1">
+        <v>13</v>
+      </c>
+      <c r="P96" s="1">
+        <v>14</v>
+      </c>
+      <c r="Q96" s="1">
+        <v>15</v>
+      </c>
+      <c r="R96" s="1">
+        <v>16</v>
+      </c>
+      <c r="S96" s="1">
+        <v>17</v>
+      </c>
+      <c r="T96" s="1">
+        <v>18</v>
+      </c>
+      <c r="U96" s="1">
+        <v>19</v>
+      </c>
+      <c r="V96" s="1">
+        <v>20</v>
+      </c>
+      <c r="W96" s="1">
+        <v>21</v>
+      </c>
+      <c r="X96" s="1">
+        <v>22</v>
+      </c>
+      <c r="Y96" s="1">
+        <v>23</v>
+      </c>
+      <c r="Z96" s="1">
+        <v>24</v>
+      </c>
+      <c r="AA96" s="1">
+        <v>25</v>
+      </c>
+      <c r="AB96" s="1">
+        <v>26</v>
+      </c>
+      <c r="AC96" s="1">
+        <v>27</v>
+      </c>
+      <c r="AD96" s="1">
+        <v>28</v>
+      </c>
+      <c r="AE96" s="1">
+        <v>29</v>
+      </c>
+      <c r="AF96" s="1">
+        <v>30</v>
+      </c>
+      <c r="AG96" s="1">
+        <v>31</v>
+      </c>
+      <c r="AH96" s="1">
+        <v>32</v>
+      </c>
+      <c r="AI96" s="1">
+        <v>33</v>
+      </c>
+      <c r="AJ96" s="1">
+        <v>34</v>
+      </c>
+      <c r="AK96" s="1">
+        <v>35</v>
+      </c>
+      <c r="AL96" s="1">
+        <v>36</v>
+      </c>
+      <c r="AM96" s="1">
+        <v>37</v>
+      </c>
+      <c r="AN96" s="1">
+        <v>38</v>
+      </c>
+      <c r="AO96" s="1">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="97" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B97" s="3" t="s">
+        <v>303</v>
       </c>
     </row>
   </sheetData>
@@ -5221,7 +5380,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="G6:H6 I6:J6 C9:D9 D20:S22 D15:I17 D26:G26 C25:F25 C28:Y28 C39:F39 L36 C42:J42 K50:L50 C53:O53 C56:L56 C59:I59 J59:P59 C62:F62 C65:I65 C71:E71 C77:I77 C80:K80 C68:F68 E89:M89 C92:E92" twoDigitTextYear="1"/>
+    <ignoredError sqref="G6:H6 I6:J6 C9:D9 D20:S22 D15:I17 D26:G26 C25:F25 C28:Y28 C39:F39 L36 C42:J42 K50:L50 C53:O53 C56:L56 C59:I59 J59:P59 C62:F62 C65:I65 C71:E71 C77:I77 C80:K80 C68:F68 E89:M89 C92:E92 C95:G95" twoDigitTextYear="1"/>
     <ignoredError sqref="C26 C15:C17 C20:C22" twoDigitTextYear="1" numberStoredAsText="1"/>
     <ignoredError sqref="C18:C19 C23:C24 AL21 C34:K34 C72 C75:L75" numberStoredAsText="1"/>
   </ignoredErrors>

</xml_diff>